<commit_message>
HTM Output files checkin
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite TaxMonth2CSBRNTK50PercentRegulatory201819.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite TaxMonth2CSBRNTK50PercentRegulatory201819.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\git\XCDHR_Payroll\Salesforce_Core_Framework\src\main\java\com\test\xcdhr\Salesforce_Core_Framework1\salesforce_XLS_Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\2018-19 Test Plan for TAX,NI,Socttish Tax\201819 Payroll Tax Module Input excel files - Correct files as all parameters are introduced\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="390" yWindow="330" windowWidth="14340" windowHeight="4215" activeTab="2"/>
+    <workbookView activeTab="3" windowHeight="7530" windowWidth="20490" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="first" sheetId="1" r:id="rId1"/>
-    <sheet name="GeneralTaxRateMonthly" sheetId="2" r:id="rId2"/>
-    <sheet name="ProcessPayrollForMonthlyTax" sheetId="4" r:id="rId3"/>
-    <sheet name="TestReports" sheetId="5" r:id="rId4"/>
+    <sheet name="first" r:id="rId1" sheetId="1"/>
+    <sheet name="GeneralTaxRateMonthly" r:id="rId2" sheetId="2"/>
+    <sheet name="ProcessPayrollForMonthlyTax" r:id="rId3" sheetId="4"/>
+    <sheet name="TestReports" r:id="rId4" sheetId="5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="62">
   <si>
     <t>TC</t>
   </si>
@@ -214,6 +214,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -281,48 +282,48 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="2">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="2" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -339,10 +340,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -377,7 +378,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -429,7 +430,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -534,7 +535,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -543,13 +544,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -559,7 +560,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -568,7 +569,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -577,7 +578,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -587,12 +588,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -623,7 +624,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -642,7 +643,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -654,7 +655,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -663,10 +664,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="38.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="33.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="38.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="33.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -683,7 +684,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -697,7 +698,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -740,25 +741,25 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="3" max="4" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -787,7 +788,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="5" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="16.149999999999999" r="2" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>22</v>
       </c>
@@ -813,7 +814,7 @@
       <c r="L2" s="6"/>
       <c r="M2" s="7"/>
     </row>
-    <row r="3" spans="1:13" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="30" r="3" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>48</v>
       </c>
@@ -834,7 +835,7 @@
       </c>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:13" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="30" r="4" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>23</v>
       </c>
@@ -855,7 +856,7 @@
       </c>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="1:13" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="30" r="5" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>24</v>
       </c>
@@ -876,7 +877,7 @@
       </c>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="1:13" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="30" r="6" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>25</v>
       </c>
@@ -897,7 +898,7 @@
       </c>
       <c r="G6" s="6"/>
     </row>
-    <row r="7" spans="1:13" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="30" r="7" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>26</v>
       </c>
@@ -918,7 +919,7 @@
       </c>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="1:13" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="30" r="8" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>49</v>
       </c>
@@ -939,7 +940,7 @@
       </c>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="1:13" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="30" r="9" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>27</v>
       </c>
@@ -960,7 +961,7 @@
       </c>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:13" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="30" r="10" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>28</v>
       </c>
@@ -981,7 +982,7 @@
       </c>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="1:13" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="30" r="11" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>29</v>
       </c>
@@ -1002,7 +1003,7 @@
       </c>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="1:13" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="30" r="12" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>50</v>
       </c>
@@ -1023,7 +1024,7 @@
       </c>
       <c r="G12" s="6"/>
     </row>
-    <row r="13" spans="1:13" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="30" r="13" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>51</v>
       </c>
@@ -1045,30 +1046,30 @@
       <c r="G13" s="6"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD23"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="36.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="49.7109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="53.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="39.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="36.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="28.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="49.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -1112,7 +1113,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="5" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>46</v>
       </c>
@@ -1147,7 +1148,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="45" r="3" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>46</v>
       </c>
@@ -1182,7 +1183,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="45" r="4" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>46</v>
       </c>
@@ -1217,7 +1218,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="45" r="5" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>46</v>
       </c>
@@ -1252,7 +1253,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="45" r="6" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>46</v>
       </c>
@@ -1287,7 +1288,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="45" r="7" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>46</v>
       </c>
@@ -1322,7 +1323,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="45" r="8" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>46</v>
       </c>
@@ -1357,7 +1358,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="45" r="9" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>46</v>
       </c>
@@ -1392,7 +1393,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="45" r="10" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>46</v>
       </c>
@@ -1427,7 +1428,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="45" r="11" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>46</v>
       </c>
@@ -1462,7 +1463,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="45" r="12" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>46</v>
       </c>
@@ -1497,7 +1498,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="45" r="13" s="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>46</v>
       </c>
@@ -1534,33 +1535,33 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
-    <hyperlink ref="A3:A13" r:id="rId2" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
+    <hyperlink display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" r:id="rId1" ref="A2"/>
+    <hyperlink display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" r:id="rId2" ref="A3:A13"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="38" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="44.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="38.42578125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17.85546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="24.42578125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="53.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="38.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="44.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="28.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="38.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="24.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -1607,7 +1608,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="5" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="70.5" r="2" s="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>46</v>
       </c>
@@ -1647,9 +1648,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
+    <hyperlink display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>